<commit_message>
CLT now updates all values ABD and abd matrices correctly!
</commit_message>
<xml_diff>
--- a/classical_laminate_theory/CLT_input_ply_mat_data/gurit_data_sheets.xlsx
+++ b/classical_laminate_theory/CLT_input_ply_mat_data/gurit_data_sheets.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\292255A\Documents\GitHub\cmt_composite_toolbox\classical_laminate_theory\CLT_input_ply_mat_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_composite_toolbox\classical_laminate_theory\CLT_input_ply_mat_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6D3F10-956A-44D1-8C10-832458F682FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7373BF-8836-4198-944B-059AA2BF2798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -30,18 +41,9 @@
     <t>Material</t>
   </si>
   <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
     <t>v12</t>
   </si>
   <si>
-    <t>G12</t>
-  </si>
-  <si>
     <t>gurit_SE84LV_RC200T</t>
   </si>
   <si>
@@ -57,13 +59,25 @@
     <t>gurit_SE84LV_IMC150</t>
   </si>
   <si>
-    <t>t</t>
+    <t>E1 [Mpa]</t>
+  </si>
+  <si>
+    <t>E2 [Mpa]</t>
+  </si>
+  <si>
+    <t>G12 [Mpa]</t>
+  </si>
+  <si>
+    <t>t [mm]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -138,13 +152,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -428,136 +444,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>71000000000</v>
-      </c>
-      <c r="D2" s="2">
-        <v>71000000000</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>71000</v>
+      </c>
+      <c r="D2" s="5">
+        <v>71000</v>
       </c>
       <c r="E2" s="4">
         <v>0.3</v>
       </c>
-      <c r="F2" s="3">
-        <v>8430000000</v>
-      </c>
-      <c r="G2" s="2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="6">
+        <v>8430</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2">
-        <v>62000000000</v>
-      </c>
-      <c r="D3" s="2">
-        <v>59000000000</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>62000</v>
+      </c>
+      <c r="D3" s="5">
+        <v>59000</v>
       </c>
       <c r="E3" s="4">
         <v>0.3</v>
       </c>
-      <c r="F3" s="3">
-        <v>8430000000</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1.5E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="6">
+        <v>8430</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2">
-        <v>177000000000</v>
-      </c>
-      <c r="D4" s="3">
-        <v>17700000000</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>177000</v>
+      </c>
+      <c r="D4" s="6">
+        <v>17700</v>
       </c>
       <c r="E4" s="4">
         <v>0.3</v>
       </c>
-      <c r="F4" s="5">
-        <v>8000000000</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2.9999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="7">
+        <v>8000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>172000000000</v>
-      </c>
-      <c r="D5" s="3">
-        <v>17200000000</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="5">
+        <v>172000</v>
+      </c>
+      <c r="D5" s="6">
+        <v>17200</v>
       </c>
       <c r="E5" s="4">
         <v>0.3</v>
       </c>
-      <c r="F5" s="5">
-        <v>4000000000</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1.5E-3</v>
-      </c>
+      <c r="F5" s="7">
+        <v>4000</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>